<commit_message>
maze_creator & LABIBI update for rezone
Signed-off-by: Quentin Booster <296188@supinfo.com>
</commit_message>
<xml_diff>
--- a/LABIBI.xlsx
+++ b/LABIBI.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Quentin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Quentin\Desktop\1ARC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40001_{E8E4E026-62FD-41B7-90DB-891DCF519BCF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FAFAF26-DF3B-43C9-9E6A-45C813DE8D96}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5676"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5676" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="4">
-  <si>
-    <t>II</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="6">
   <si>
     <t>DD</t>
   </si>
@@ -38,11 +35,20 @@
   <si>
     <t>x</t>
   </si>
+  <si>
+    <t>1case = 1 unit</t>
+  </si>
+  <si>
+    <t>csvid</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -90,7 +96,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -105,6 +111,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -420,11 +429,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BI22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:BJ22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="AC17" sqref="AC17"/>
+      <selection activeCell="AL17" activeCellId="1" sqref="A22:X22 AL17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -432,195 +441,201 @@
     <col min="1" max="1" width="6.33203125" customWidth="1"/>
     <col min="2" max="30" width="3.5546875" customWidth="1"/>
     <col min="31" max="60" width="4.109375" customWidth="1"/>
+    <col min="61" max="61" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
+    <row r="1" spans="1:62" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AS1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AT1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AU1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AV1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AW1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AX1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AY1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AZ1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BA1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BB1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BC1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BD1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BE1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BF1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BG1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BH1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="BI1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:62" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -648,16 +663,19 @@
       <c r="AA2" s="2"/>
       <c r="AB2" s="2"/>
       <c r="AC2" s="2"/>
-      <c r="AD2" s="1"/>
-      <c r="BH2" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="2"/>
+      <c r="AD2" s="2"/>
+      <c r="AE2" s="1"/>
+      <c r="BI2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:62" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -685,16 +703,19 @@
       <c r="AA3" s="2"/>
       <c r="AB3" s="2"/>
       <c r="AC3" s="2"/>
-      <c r="AD3" s="1"/>
-      <c r="BH3" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="2"/>
+      <c r="AD3" s="2"/>
+      <c r="AE3" s="1"/>
+      <c r="BI3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:62" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -722,16 +743,19 @@
       <c r="AA4" s="2"/>
       <c r="AB4" s="2"/>
       <c r="AC4" s="2"/>
-      <c r="AD4" s="1"/>
-      <c r="BH4" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="2"/>
+      <c r="AD4" s="2"/>
+      <c r="AE4" s="1"/>
+      <c r="BI4" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:62" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -759,16 +783,22 @@
       <c r="AA5" s="2"/>
       <c r="AB5" s="2"/>
       <c r="AC5" s="2"/>
-      <c r="AD5" s="1"/>
-      <c r="BH5" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="2"/>
+      <c r="AD5" s="2"/>
+      <c r="AE5" s="1"/>
+      <c r="BI5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="BJ5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:62" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -796,16 +826,19 @@
       <c r="AA6" s="2"/>
       <c r="AB6" s="2"/>
       <c r="AC6" s="2"/>
-      <c r="AD6" s="1"/>
-      <c r="BH6" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="2"/>
+      <c r="AD6" s="2"/>
+      <c r="AE6" s="1"/>
+      <c r="BI6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:62" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -833,16 +866,20 @@
       <c r="AA7" s="2"/>
       <c r="AB7" s="2"/>
       <c r="AC7" s="2"/>
-      <c r="AD7" s="1"/>
-      <c r="BH7" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="2"/>
+      <c r="AD7" s="2"/>
+      <c r="AE7" s="1"/>
+      <c r="BI7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="BJ7" s="2"/>
+    </row>
+    <row r="8" spans="1:62" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -870,16 +907,19 @@
       <c r="AA8" s="2"/>
       <c r="AB8" s="2"/>
       <c r="AC8" s="2"/>
-      <c r="AD8" s="1"/>
-      <c r="BH8" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="2"/>
+      <c r="AD8" s="2"/>
+      <c r="AE8" s="1"/>
+      <c r="BI8" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:62" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -907,17 +947,19 @@
       <c r="AA9" s="2"/>
       <c r="AB9" s="2"/>
       <c r="AC9" s="2"/>
-      <c r="AD9" s="1"/>
-      <c r="BH9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="BI9" s="2"/>
-    </row>
-    <row r="10" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="2"/>
+      <c r="AD9" s="2"/>
+      <c r="AE9" s="1"/>
+      <c r="BI9" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:62" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -945,16 +987,19 @@
       <c r="AA10" s="2"/>
       <c r="AB10" s="2"/>
       <c r="AC10" s="2"/>
-      <c r="AD10" s="1"/>
-      <c r="BH10" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" s="2"/>
+      <c r="AD10" s="2"/>
+      <c r="AE10" s="1"/>
+      <c r="BI10" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:62" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -982,16 +1027,19 @@
       <c r="AA11" s="2"/>
       <c r="AB11" s="2"/>
       <c r="AC11" s="2"/>
-      <c r="AD11" s="1"/>
-      <c r="BH11" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" s="2"/>
+      <c r="AD11" s="2"/>
+      <c r="AE11" s="1"/>
+      <c r="BI11" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:62" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -1019,16 +1067,19 @@
       <c r="AA12" s="2"/>
       <c r="AB12" s="2"/>
       <c r="AC12" s="2"/>
-      <c r="AD12" s="1"/>
-      <c r="BH12" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" s="2"/>
+      <c r="AD12" s="2"/>
+      <c r="AE12" s="1"/>
+      <c r="BI12" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:62" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -1056,16 +1107,19 @@
       <c r="AA13" s="2"/>
       <c r="AB13" s="2"/>
       <c r="AC13" s="2"/>
-      <c r="AD13" s="1"/>
-      <c r="BH13" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14" s="2"/>
+      <c r="AD13" s="2"/>
+      <c r="AE13" s="1"/>
+      <c r="BI13" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:62" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -1093,16 +1147,19 @@
       <c r="AA14" s="2"/>
       <c r="AB14" s="2"/>
       <c r="AC14" s="2"/>
-      <c r="AD14" s="1"/>
-      <c r="BH14" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B15" s="2"/>
+      <c r="AD14" s="2"/>
+      <c r="AE14" s="1"/>
+      <c r="BI14" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:62" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -1130,16 +1187,19 @@
       <c r="AA15" s="2"/>
       <c r="AB15" s="2"/>
       <c r="AC15" s="2"/>
-      <c r="AD15" s="1"/>
-      <c r="BH15" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16" s="2"/>
+      <c r="AD15" s="2"/>
+      <c r="AE15" s="1"/>
+      <c r="BI15" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:62" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -1152,49 +1212,60 @@
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
       <c r="N16" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R16" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="S16" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="T16" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="U16" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="V16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="W16" s="2"/>
-      <c r="X16" s="2"/>
-      <c r="Y16" s="2"/>
-      <c r="Z16" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="W16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="X16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z16" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="AA16" s="2"/>
       <c r="AB16" s="2"/>
       <c r="AC16" s="2"/>
-      <c r="AD16" s="1"/>
-      <c r="BH16" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B17" s="2"/>
+      <c r="AD16" s="2"/>
+      <c r="AE16" s="1"/>
+      <c r="BI16" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -1207,39 +1278,37 @@
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
       <c r="N17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O17" s="1"/>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="U17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="V17" s="2"/>
+      <c r="W17" s="6"/>
+      <c r="Z17" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="O17" s="2"/>
-      <c r="P17" s="2"/>
-      <c r="Q17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="R17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="S17" s="2"/>
-      <c r="T17" s="2"/>
-      <c r="U17" s="2"/>
-      <c r="V17" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="W17" s="2"/>
-      <c r="X17" s="2"/>
-      <c r="Y17" s="2"/>
-      <c r="Z17" s="2"/>
       <c r="AA17" s="2"/>
       <c r="AB17" s="2"/>
       <c r="AC17" s="2"/>
-      <c r="AD17" s="1"/>
-      <c r="BH17" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18" s="2"/>
+      <c r="AD17" s="2"/>
+      <c r="AE17" s="1"/>
+      <c r="BI17" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -1252,37 +1321,37 @@
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
       <c r="N18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O18" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="O18" s="1"/>
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
-      <c r="R18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="S18" s="2"/>
-      <c r="T18" s="2"/>
-      <c r="U18" s="2"/>
-      <c r="V18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="W18" s="2"/>
-      <c r="X18" s="2"/>
-      <c r="Y18" s="2"/>
-      <c r="Z18" s="2"/>
+      <c r="R18" s="2"/>
+      <c r="S18" s="1"/>
+      <c r="U18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="V18" s="2"/>
+      <c r="W18" s="1"/>
+      <c r="Z18" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="AA18" s="2"/>
       <c r="AB18" s="2"/>
       <c r="AC18" s="2"/>
-      <c r="AD18" s="1"/>
-      <c r="BH18" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B19" s="2"/>
+      <c r="AD18" s="2"/>
+      <c r="AE18" s="1"/>
+      <c r="BI18" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -1295,43 +1364,44 @@
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
       <c r="N19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O19" s="2"/>
-      <c r="P19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q19" s="2"/>
-      <c r="R19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="S19" s="2"/>
-      <c r="T19" s="1" t="s">
-        <v>0</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="O19" s="1"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="R19" s="2"/>
+      <c r="S19" s="1"/>
       <c r="U19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="V19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="W19" s="2"/>
-      <c r="X19" s="2"/>
-      <c r="Y19" s="2"/>
-      <c r="Z19" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="V19" s="1"/>
+      <c r="X19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z19" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="AA19" s="2"/>
       <c r="AB19" s="2"/>
       <c r="AC19" s="2"/>
-      <c r="AD19" s="1"/>
-      <c r="BH19" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B20" s="2"/>
+      <c r="AD19" s="2"/>
+      <c r="AE19" s="1"/>
+      <c r="BI19" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -1344,41 +1414,41 @@
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
       <c r="N20" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O20" s="2"/>
-      <c r="P20" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="2"/>
-      <c r="R20" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="S20" s="2"/>
-      <c r="T20" s="2"/>
-      <c r="U20" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="V20" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="W20" s="2"/>
-      <c r="X20" s="2"/>
-      <c r="Y20" s="2"/>
-      <c r="Z20" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="O20" s="1"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="R20" s="2"/>
+      <c r="S20" s="1"/>
+      <c r="U20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="V20" s="5"/>
+      <c r="Y20" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z20" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="AA20" s="2"/>
       <c r="AB20" s="2"/>
       <c r="AC20" s="2"/>
-      <c r="AD20" s="1"/>
-      <c r="BH20" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B21" s="2"/>
+      <c r="AD20" s="2"/>
+      <c r="AE20" s="1"/>
+      <c r="BI20" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -1391,214 +1461,218 @@
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
       <c r="N21" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O21" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="P21" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q21" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="P21" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q21" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="R21" s="2"/>
       <c r="S21" s="2"/>
       <c r="T21" s="2"/>
-      <c r="U21" s="5"/>
-      <c r="V21" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="W21" s="2"/>
-      <c r="X21" s="2"/>
-      <c r="Y21" s="2"/>
-      <c r="Z21" s="2"/>
+      <c r="U21" s="2"/>
+      <c r="V21" s="5"/>
+      <c r="W21" s="1"/>
+      <c r="Z21" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="AA21" s="2"/>
       <c r="AB21" s="2"/>
       <c r="AC21" s="2"/>
-      <c r="AD21" s="1"/>
-      <c r="BH21" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
-        <v>0</v>
+      <c r="AD21" s="2"/>
+      <c r="AE21" s="1"/>
+      <c r="BI21" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="S22" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="T22" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="U22" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="V22" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="W22" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="X22" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Y22" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Z22" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AA22" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AB22" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AC22" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AD22" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AE22" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AF22" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AG22" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AH22" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AI22" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AJ22" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AK22" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AL22" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AM22" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AN22" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AO22" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AP22" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AQ22" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AR22" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AS22" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AT22" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AU22" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AV22" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AW22" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AX22" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AY22" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AZ22" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BA22" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BB22" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BC22" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BD22" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BE22" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BF22" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BG22" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BH22" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="BI22" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working draw and object interract in redzone (missing the "And" statement in "testpos" for detecting object with lines and not only column)
Signed-off-by: Quentin Booster <296188@supinfo.com>
</commit_message>
<xml_diff>
--- a/LABIBI.xlsx
+++ b/LABIBI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Quentin\Desktop\1ARC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FAFAF26-DF3B-43C9-9E6A-45C813DE8D96}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65AACD90-7C4B-491A-9905-D2875425DDC8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5676" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -432,8 +432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BJ22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="AL17" activeCellId="1" sqref="A22:X22 AL17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="AL24" sqref="AL24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
version avec menu (not working) boucle infini inpossible de quitter le jeu
Signed-off-by: Quentin Booster <296188@supinfo.com>
</commit_message>
<xml_diff>
--- a/LABIBI.xlsx
+++ b/LABIBI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Quentin\Desktop\1ARC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65AACD90-7C4B-491A-9905-D2875425DDC8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10E39603-D8B2-4075-BC30-691B7532F319}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5676" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="7">
   <si>
     <t>DD</t>
   </si>
@@ -36,13 +36,16 @@
     <t>x</t>
   </si>
   <si>
-    <t>1case = 1 unit</t>
-  </si>
-  <si>
     <t>csvid</t>
   </si>
   <si>
     <t>I</t>
+  </si>
+  <si>
+    <t>*message*</t>
+  </si>
+  <si>
+    <t>Press</t>
   </si>
 </sst>
 </file>
@@ -432,8 +435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BJ22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="AL24" sqref="AL24"/>
+    <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="AI22" sqref="AI22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -446,195 +449,198 @@
   <sheetData>
     <row r="1" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AS1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AT1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AU1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AV1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AW1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AX1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AY1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AZ1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BA1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BB1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BC1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BD1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BE1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BF1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BG1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BH1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BI1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="BJ1" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -666,15 +672,15 @@
       <c r="AD2" s="2"/>
       <c r="AE2" s="1"/>
       <c r="BI2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -706,15 +712,15 @@
       <c r="AD3" s="2"/>
       <c r="AE3" s="1"/>
       <c r="BI3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -746,15 +752,15 @@
       <c r="AD4" s="2"/>
       <c r="AE4" s="1"/>
       <c r="BI4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -786,18 +792,15 @@
       <c r="AD5" s="2"/>
       <c r="AE5" s="1"/>
       <c r="BI5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="BJ5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -829,15 +832,18 @@
       <c r="AD6" s="2"/>
       <c r="AE6" s="1"/>
       <c r="BI6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="BJ6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -869,16 +875,18 @@
       <c r="AD7" s="2"/>
       <c r="AE7" s="1"/>
       <c r="BI7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="BJ7" t="s">
         <v>5</v>
       </c>
-      <c r="BJ7" s="2"/>
     </row>
     <row r="8" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -910,15 +918,15 @@
       <c r="AD8" s="2"/>
       <c r="AE8" s="1"/>
       <c r="BI8" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -950,15 +958,15 @@
       <c r="AD9" s="2"/>
       <c r="AE9" s="1"/>
       <c r="BI9" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -990,15 +998,15 @@
       <c r="AD10" s="2"/>
       <c r="AE10" s="1"/>
       <c r="BI10" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -1030,15 +1038,15 @@
       <c r="AD11" s="2"/>
       <c r="AE11" s="1"/>
       <c r="BI11" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -1070,15 +1078,15 @@
       <c r="AD12" s="2"/>
       <c r="AE12" s="1"/>
       <c r="BI12" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -1110,15 +1118,15 @@
       <c r="AD13" s="2"/>
       <c r="AE13" s="1"/>
       <c r="BI13" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -1150,15 +1158,15 @@
       <c r="AD14" s="2"/>
       <c r="AE14" s="1"/>
       <c r="BI14" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -1190,15 +1198,15 @@
       <c r="AD15" s="2"/>
       <c r="AE15" s="1"/>
       <c r="BI15" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -1212,43 +1220,43 @@
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
       <c r="N16" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="R16" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="S16" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="T16" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="U16" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="V16" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="W16" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="X16" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Y16" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Z16" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AA16" s="2"/>
       <c r="AB16" s="2"/>
@@ -1256,15 +1264,15 @@
       <c r="AD16" s="2"/>
       <c r="AE16" s="1"/>
       <c r="BI16" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:61" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -1278,7 +1286,7 @@
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
       <c r="N17" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O17" s="1"/>
       <c r="P17" s="2"/>
@@ -1286,7 +1294,7 @@
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
       <c r="U17" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="V17" s="2"/>
       <c r="W17" s="6"/>
@@ -1299,15 +1307,15 @@
       <c r="AD17" s="2"/>
       <c r="AE17" s="1"/>
       <c r="BI17" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:61" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -1321,7 +1329,7 @@
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
       <c r="N18" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O18" s="1"/>
       <c r="P18" s="2"/>
@@ -1329,12 +1337,12 @@
       <c r="R18" s="2"/>
       <c r="S18" s="1"/>
       <c r="U18" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="V18" s="2"/>
       <c r="W18" s="1"/>
       <c r="Z18" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AA18" s="2"/>
       <c r="AB18" s="2"/>
@@ -1342,15 +1350,15 @@
       <c r="AD18" s="2"/>
       <c r="AE18" s="1"/>
       <c r="BI18" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:61" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -1364,27 +1372,27 @@
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
       <c r="N19" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O19" s="1"/>
       <c r="P19" s="2"/>
       <c r="Q19" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="R19" s="2"/>
       <c r="S19" s="1"/>
       <c r="U19" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="V19" s="1"/>
       <c r="X19" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Y19" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Z19" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AA19" s="2"/>
       <c r="AB19" s="2"/>
@@ -1392,15 +1400,15 @@
       <c r="AD19" s="2"/>
       <c r="AE19" s="1"/>
       <c r="BI19" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:61" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -1414,24 +1422,24 @@
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
       <c r="N20" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O20" s="1"/>
       <c r="P20" s="2"/>
       <c r="Q20" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="R20" s="2"/>
       <c r="S20" s="1"/>
       <c r="U20" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="V20" s="5"/>
       <c r="Y20" s="3" t="s">
         <v>1</v>
       </c>
       <c r="Z20" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AA20" s="2"/>
       <c r="AB20" s="2"/>
@@ -1439,15 +1447,15 @@
       <c r="AD20" s="2"/>
       <c r="AE20" s="1"/>
       <c r="BI20" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:61" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -1461,7 +1469,7 @@
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
       <c r="N21" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O21" s="1" t="s">
         <v>2</v>
@@ -1470,7 +1478,7 @@
         <v>2</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="R21" s="2"/>
       <c r="S21" s="2"/>
@@ -1479,7 +1487,7 @@
       <c r="V21" s="5"/>
       <c r="W21" s="1"/>
       <c r="Z21" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AA21" s="2"/>
       <c r="AB21" s="2"/>
@@ -1487,192 +1495,192 @@
       <c r="AD21" s="2"/>
       <c r="AE21" s="1"/>
       <c r="BI21" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:61" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="S22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="T22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="U22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="V22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="W22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="X22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Y22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Z22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AA22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AB22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AC22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AD22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AE22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AF22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AG22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AH22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AI22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AJ22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AK22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AL22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AM22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AN22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AO22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AP22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AQ22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AR22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AS22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AT22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AU22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AV22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AW22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AX22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AY22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AZ22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BA22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BB22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BC22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BD22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BE22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BF22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BG22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BH22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BI22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>